<commit_message>
Fix "Possibly not at 100%" QC reports
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_prior_year_card_code_5s_dweldat.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_prior_year_card_code_5s_dweldat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83328ED-0F33-4CA0-BA78-79D27774419B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655CCB28-6F7C-4CC2-9FB1-711CAE25FBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="4455" windowWidth="21600" windowHeight="11295" xr2:uid="{F86E03EA-3BEB-4D35-8C8E-3F43C895C1B8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F86E03EA-3BEB-4D35-8C8E-3F43C895C1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -203,11 +203,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,9 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C9F7A4-E508-400A-BB6E-1E0697A206D7}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,8 +545,8 @@
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
@@ -604,10 +608,10 @@
       <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="2" t="s">

</xml_diff>